<commit_message>
make subfunctions and feedback implementation
</commit_message>
<xml_diff>
--- a/model/data/beerwiser/xlsx/beerwiser.xlsx
+++ b/model/data/beerwiser/xlsx/beerwiser.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tdijk004/Documents/tRBS/open source/trbs/model/data/beerwiser/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mverdaasdo001/Documents/RBS_open_source_test/trbs/model/data/beerwiser/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{468B641F-C12C-FB44-9437-884644042C27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFAE3F05-47B4-0F4A-A6D7-56EE2674AC7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="configurations" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="60">
   <si>
     <t>configuration</t>
   </si>
@@ -202,6 +202,12 @@
   </si>
   <si>
     <t>squeezed *</t>
+  </si>
+  <si>
+    <t>strategic_challenge</t>
+  </si>
+  <si>
+    <t>How to ensure a sustainable production process?</t>
   </si>
 </sst>
 </file>
@@ -565,10 +571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -587,6 +593,14 @@
       </c>
       <c r="B2">
         <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1265,8 +1279,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R36" sqref="R36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>